<commit_message>
Add test for skipping empty columns
</commit_message>
<xml_diff>
--- a/spec/fixtures/balls_blank_columns.xlsx
+++ b/spec/fixtures/balls_blank_columns.xlsx
@@ -5,25 +5,30 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="balls" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>color</t>
+    <t xml:space="preserve">color</t>
   </si>
   <si>
-    <t>red</t>
+    <t xml:space="preserve">red</t>
   </si>
   <si>
-    <t>blue</t>
+    <t xml:space="preserve">blue</t>
   </si>
 </sst>
 </file>
@@ -31,7 +36,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="4">
@@ -125,95 +130,94 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AG3"/>
+  <dimension ref="B1:AG3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.46428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.12755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.37755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.1887755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.15816326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.1887755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.2091836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.6071428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.734693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.71428571428571"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.98469387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.76530612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.9030612244898"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="31.1632653061224"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="20.1836734693878"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.1275510204082"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="47.1377551020408"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="21.7142857142857"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="22.1275510204082"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="155.107142857143"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="23.2448979591837"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="22.1275510204082"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="20.3316326530612"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="21.1581632653061"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="25.0561224489796"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="23.9387755102041"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="31.5765306122449"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="21.5816326530612"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="25.7448979591837"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="26.4387755102041"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="23.5255102040816"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="26.5765306122449"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="24.0714285714286"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="9.07142857142857"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.8010204081633"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="13.9336734693878"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="14.4897959183673"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.9336734693878"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="15.3265306122449"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="14.3520408163265"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="16.2959183673469"/>
-    <col collapsed="false" hidden="false" max="44" min="43" style="0" width="20.4642857142857"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="18.8010204081633"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="17.2704081632653"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="50" min="49" style="0" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="52" min="52" style="0" width="14.9030612244898"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="18.5204081632653"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="23.5255102040816"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="28.9438775510204"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="30.8877551020408"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="23.5255102040816"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="25.469387755102"/>
-    <col collapsed="false" hidden="false" max="59" min="59" style="0" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="20.4642857142857"/>
-    <col collapsed="false" hidden="false" max="61" min="61" style="0" width="18.5204081632653"/>
-    <col collapsed="false" hidden="false" max="62" min="62" style="0" width="23.9387755102041"/>
-    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="21.5816326530612"/>
-    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="65" min="65" style="0" width="25.469387755102"/>
-    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="15.3265306122449"/>
-    <col collapsed="false" hidden="false" max="67" min="67" style="0" width="21.8520408163265"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="21.1581632653061"/>
-    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="19.3571428571429"/>
-    <col collapsed="false" hidden="false" max="70" min="70" style="0" width="22.9642857142857"/>
-    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="22.1275510204082"/>
-    <col collapsed="false" hidden="false" max="72" min="72" style="0" width="22.5510204081633"/>
-    <col collapsed="false" hidden="false" max="73" min="73" style="0" width="21.9948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="74" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="5.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="6.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="20.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="22.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="47.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="22.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="155.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="23.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="22.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="20.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="21.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="25.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="23.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="31.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="21.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="25.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="26.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="23.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="26.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="24.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="9.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="18.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="14.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="15.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="43" style="0" width="20.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="18.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="17.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="49" style="0" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="0" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="0" width="18.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="0" width="23.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="0" width="28.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="0" width="30.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="0" width="23.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="0" width="25.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="0" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="0" width="20.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="0" width="18.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="0" width="23.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="0" width="21.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="0" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="0" width="25.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="0" width="15.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="0" width="21.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="0" width="21.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="69" style="0" width="19.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="0" width="22.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="71" min="71" style="0" width="22.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="72" min="72" style="0" width="22.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="73" min="73" style="0" width="21.99"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="74" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="B1" s="0" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>1</v>
       </c>
       <c r="AD2" s="1"/>
@@ -222,7 +226,7 @@
       <c r="AG2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>2</v>
       </c>
       <c r="AD3" s="1"/>
@@ -233,7 +237,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>